<commit_message>
#commit change export data, update LCL export
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Commission-OPS-VND.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Commission-OPS-VND.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>COMMISSION PAYMENT REQUEST</t>
   </si>
@@ -237,7 +237,37 @@
     <t>{ManagerDep}</t>
   </si>
   <si>
-    <t>{Total}</t>
+    <t>{Total1}</t>
+  </si>
+  <si>
+    <t>{Total2}</t>
+  </si>
+  <si>
+    <t>{Total3}</t>
+  </si>
+  <si>
+    <t>{Total4}</t>
+  </si>
+  <si>
+    <t>{Total5}</t>
+  </si>
+  <si>
+    <t>{Total6}</t>
+  </si>
+  <si>
+    <t>{Total7}</t>
+  </si>
+  <si>
+    <t>{Total8}</t>
+  </si>
+  <si>
+    <t>{Total9}</t>
+  </si>
+  <si>
+    <t>{Total10}</t>
+  </si>
+  <si>
+    <t>{Total11}</t>
   </si>
 </sst>
 </file>
@@ -615,17 +645,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,10 +657,39 @@
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -931,7 +979,7 @@
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1006,50 +1054,50 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:19" s="3" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
     </row>
     <row r="9" spans="1:19" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
     </row>
     <row r="10" spans="1:19" s="3" customFormat="1">
       <c r="A10" s="1"/>
@@ -1172,57 +1220,57 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="23.25" customHeight="1">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="51"/>
-      <c r="F13" s="42" t="s">
+      <c r="E13" s="46"/>
+      <c r="F13" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="53" t="s">
+      <c r="I13" s="49"/>
+      <c r="J13" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="54" t="s">
+      <c r="K13" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="L13" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="N13" s="44" t="s">
+      <c r="N13" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="O13" s="44" t="s">
+      <c r="O13" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="P13" s="44" t="s">
+      <c r="P13" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="Q13" s="46" t="s">
+      <c r="Q13" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="R13" s="46" t="s">
+      <c r="R13" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="S13" s="44" t="s">
+      <c r="S13" s="52" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1243,34 +1291,34 @@
         <v>0</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="P14" s="15" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="R14" s="15" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="5.25" customHeight="1"/>
@@ -1337,8 +1385,8 @@
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
       <c r="L18" s="17"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
       <c r="O18" s="19"/>
       <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
@@ -1361,8 +1409,8 @@
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
@@ -1431,8 +1479,8 @@
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
       <c r="O22" s="26"/>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>

</xml_diff>